<commit_message>
Update projektcharter och tidrapporter.
</commit_message>
<xml_diff>
--- a/Dokument/Tidsrapportering/Tidrapport_Emil.xlsx
+++ b/Dokument/Tidsrapportering/Tidrapport_Emil.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jimmy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\ProjectC4\Dokument\Tidsrapportering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Översikt" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
   <si>
     <t>Tidrapport sammanfattning</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Emil Sandgren</t>
+  </si>
+  <si>
+    <t>Planering, dokumentskapande.</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -886,7 +889,7 @@
       </c>
       <c r="D10" s="17">
         <f>Mars!C42</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>4</v>
@@ -953,7 +956,7 @@
       </c>
       <c r="D16" s="19">
         <f>SUM(D10:D12)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>4</v>
@@ -975,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1051,7 @@
       </c>
       <c r="C8" s="28" t="str">
         <f>SUM(C11:C41) &amp; " h"</f>
-        <v>0 h</v>
+        <v>4 h</v>
       </c>
       <c r="D8" s="22"/>
     </row>
@@ -1172,8 +1175,12 @@
       <c r="B26" s="32">
         <v>42079</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
+      <c r="C26" s="35">
+        <v>4</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="32">
@@ -1286,7 +1293,7 @@
       </c>
       <c r="C42" s="40">
         <f>SUM(C11:C41)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D42" s="41" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
UPDATE: projektplan, tidrapport, och uppdelat gantt-schema
</commit_message>
<xml_diff>
--- a/Dokument/Tidsrapportering/Tidrapport_Emil.xlsx
+++ b/Dokument/Tidsrapportering/Tidrapport_Emil.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Översikt" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="21">
   <si>
     <t>Tidrapport sammanfattning</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Planering, dokumentskapande.</t>
+  </si>
+  <si>
+    <t>Testmall och skisser</t>
   </si>
 </sst>
 </file>
@@ -810,22 +813,22 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="21.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.7265625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="21.453125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.5">
       <c r="B3" s="5"/>
       <c r="C3" s="6" t="s">
         <v>0</v>
@@ -833,13 +836,13 @@
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="5"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="5"/>
       <c r="C5" s="9" t="s">
         <v>1</v>
@@ -849,7 +852,7 @@
       </c>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="5"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
@@ -859,7 +862,7 @@
       </c>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="5"/>
       <c r="C7" s="9" t="s">
         <v>2</v>
@@ -869,19 +872,19 @@
       </c>
       <c r="E7" s="11"/>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="14"/>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9" s="5"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
       <c r="C10" s="16" t="str">
         <f>Mars!C7</f>
@@ -889,13 +892,13 @@
       </c>
       <c r="D10" s="17">
         <f>Mars!C42</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="16" t="str">
         <f>April!C7</f>
@@ -909,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="5"/>
       <c r="C12" s="16" t="str">
         <f>Maj!C7</f>
@@ -923,7 +926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="16" t="str">
         <f>Juni!C7</f>
@@ -937,32 +940,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="5"/>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="42"/>
       <c r="C15" s="43"/>
       <c r="D15" s="44"/>
       <c r="E15" s="45"/>
     </row>
-    <row r="16" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
       <c r="C16" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="19">
         <f>SUM(D10:D12)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
@@ -978,30 +981,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1011,7 +1014,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1024,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
@@ -1031,12 +1034,12 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="25"/>
       <c r="C6" s="10"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
@@ -1045,17 +1048,17 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>SUM(C11:C41) &amp; " h"</f>
-        <v>4 h</v>
+        <v>8 h</v>
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
@@ -1066,112 +1069,112 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="32">
         <v>42064</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>42065</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>42066</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="32">
         <v>42067</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="32">
         <v>42068</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="32">
         <v>42069</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="32">
         <v>42070</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>42071</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>42072</v>
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="32">
         <v>42073</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="36"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="32">
         <v>42074</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="32">
         <v>42075</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="36"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="32">
         <v>42076</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="32">
         <v>42077</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="32">
         <v>42078</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="32">
         <v>42079</v>
       </c>
@@ -1182,118 +1185,122 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="32">
         <v>42080</v>
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="32">
         <v>42081</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="32">
         <v>42082</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="35">
+        <v>4</v>
+      </c>
+      <c r="D29" s="36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="32">
         <v>42083</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="36"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="32">
         <v>42084</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="32">
         <v>42085</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="32">
         <v>42086</v>
       </c>
       <c r="C33" s="35"/>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="32">
         <v>42087</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="36"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="32">
         <v>42088</v>
       </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="32">
         <v>42089</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="36"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="32">
         <v>42090</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="32">
         <v>42091</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="32">
         <v>42092</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="36"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="32">
         <v>42093</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="32">
         <v>42094</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38"/>
     </row>
-    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B42" s="39" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="40">
         <f>SUM(C11:C41)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D42" s="41" t="s">
         <v>13</v>
@@ -1312,26 +1319,26 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1341,7 +1348,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
@@ -1351,7 +1358,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
@@ -1361,12 +1368,12 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="25"/>
       <c r="C6" s="10"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
@@ -1375,7 +1382,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1392,7 @@
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
@@ -1396,217 +1403,217 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="32">
         <v>42095</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>42096</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>42097</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="32">
         <v>42098</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="32">
         <v>42099</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="32">
         <v>42100</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="32">
         <v>42101</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>42102</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>42103</v>
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="32">
         <v>42104</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="36"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="32">
         <v>42105</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="32">
         <v>42106</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="36"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="32">
         <v>42107</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="32">
         <v>42108</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="32">
         <v>42109</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="32">
         <v>42110</v>
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="36"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="32">
         <v>42111</v>
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="32">
         <v>42112</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="32">
         <v>42113</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="32">
         <v>42114</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="36"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="32">
         <v>42115</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="32">
         <v>42116</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="32">
         <v>42117</v>
       </c>
       <c r="C33" s="35"/>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="32">
         <v>42118</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="36"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="32">
         <v>42119</v>
       </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="32">
         <v>42120</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="36"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="32">
         <v>42121</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="32">
         <v>42122</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="32">
         <v>42123</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="36"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="32">
         <v>42124</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
     </row>
-    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B41" s="39" t="s">
         <v>5</v>
       </c>
@@ -1631,26 +1638,26 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1660,7 +1667,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1677,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
@@ -1680,12 +1687,12 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="25"/>
       <c r="C6" s="10"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
@@ -1694,7 +1701,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1711,7 @@
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
@@ -1715,224 +1722,224 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="32">
         <v>42125</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>42126</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>42127</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="32">
         <v>42128</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="32">
         <v>42129</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="32">
         <v>42130</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="32">
         <v>42131</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>42132</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>42133</v>
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="32">
         <v>42134</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="36"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="32">
         <v>42135</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="32">
         <v>42136</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="36"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="32">
         <v>42137</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="32">
         <v>42138</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="32">
         <v>42139</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="32">
         <v>42140</v>
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="36"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="32">
         <v>42141</v>
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="32">
         <v>42142</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="32">
         <v>42143</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="32">
         <v>42144</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="36"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="32">
         <v>42145</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="32">
         <v>42146</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="32">
         <v>42147</v>
       </c>
       <c r="C33" s="35"/>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="32">
         <v>42148</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="36"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="32">
         <v>42149</v>
       </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="32">
         <v>42150</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="36"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="32">
         <v>42151</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="32">
         <v>42152</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="32">
         <v>42153</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="36"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="32">
         <v>42154</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="32">
         <v>42155</v>
       </c>
       <c r="C41" s="37"/>
       <c r="D41" s="38"/>
     </row>
-    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B42" s="39" t="s">
         <v>5</v>
       </c>
@@ -1957,26 +1964,26 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23"/>
     </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
@@ -1986,7 +1993,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" s="25" t="s">
         <v>3</v>
       </c>
@@ -1996,7 +2003,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="25" t="s">
         <v>2</v>
       </c>
@@ -2006,12 +2013,12 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="25"/>
       <c r="C6" s="10"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
@@ -2020,7 +2027,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="27" t="s">
         <v>9</v>
       </c>
@@ -2030,7 +2037,7 @@
       </c>
       <c r="D8" s="22"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="29" t="s">
         <v>10</v>
       </c>
@@ -2041,217 +2048,217 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B11" s="32">
         <v>42156</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="34"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>42157</v>
       </c>
       <c r="C12" s="35"/>
       <c r="D12" s="36"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>42158</v>
       </c>
       <c r="C13" s="35"/>
       <c r="D13" s="36"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" s="32">
         <v>42159</v>
       </c>
       <c r="C14" s="35"/>
       <c r="D14" s="36"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" s="32">
         <v>42160</v>
       </c>
       <c r="C15" s="35"/>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B16" s="32">
         <v>42161</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="36"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="32">
         <v>42162</v>
       </c>
       <c r="C17" s="35"/>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>42163</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="36"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>42164</v>
       </c>
       <c r="C19" s="35"/>
       <c r="D19" s="36"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="32">
         <v>42165</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="36"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="32">
         <v>42166</v>
       </c>
       <c r="C21" s="35"/>
       <c r="D21" s="36"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="32">
         <v>42167</v>
       </c>
       <c r="C22" s="35"/>
       <c r="D22" s="36"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="32">
         <v>42168</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="32">
         <v>42169</v>
       </c>
       <c r="C24" s="35"/>
       <c r="D24" s="36"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="32">
         <v>42170</v>
       </c>
       <c r="C25" s="35"/>
       <c r="D25" s="36"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="32">
         <v>42171</v>
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="36"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="32">
         <v>42172</v>
       </c>
       <c r="C27" s="35"/>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="32">
         <v>42173</v>
       </c>
       <c r="C28" s="35"/>
       <c r="D28" s="36"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="32">
         <v>42174</v>
       </c>
       <c r="C29" s="35"/>
       <c r="D29" s="36"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="32">
         <v>42175</v>
       </c>
       <c r="C30" s="35"/>
       <c r="D30" s="36"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="32">
         <v>42176</v>
       </c>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="32">
         <v>42177</v>
       </c>
       <c r="C32" s="35"/>
       <c r="D32" s="36"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="32">
         <v>42178</v>
       </c>
       <c r="C33" s="35"/>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="32">
         <v>42179</v>
       </c>
       <c r="C34" s="35"/>
       <c r="D34" s="36"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="32">
         <v>42180</v>
       </c>
       <c r="C35" s="35"/>
       <c r="D35" s="36"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="32">
         <v>42181</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="36"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="32">
         <v>42182</v>
       </c>
       <c r="C37" s="35"/>
       <c r="D37" s="36"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="32">
         <v>42183</v>
       </c>
       <c r="C38" s="35"/>
       <c r="D38" s="36"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="32">
         <v>42184</v>
       </c>
       <c r="C39" s="35"/>
       <c r="D39" s="36"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="32">
         <v>42185</v>
       </c>
       <c r="C40" s="35"/>
       <c r="D40" s="36"/>
     </row>
-    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B41" s="39" t="s">
         <v>5</v>
       </c>

</xml_diff>